<commit_message>
update in db CRM
</commit_message>
<xml_diff>
--- a/Kvota/wwwroot/excel/ExcelOutputKvota.xlsx
+++ b/Kvota/wwwroot/excel/ExcelOutputKvota.xlsx
@@ -88,25 +88,13 @@
     <x:t>9898989</x:t>
   </x:si>
   <x:si>
-    <x:t>22</x:t>
+    <x:t>Analog Devices</x:t>
   </x:si>
   <x:si>
     <x:t>Cat4</x:t>
   </x:si>
   <x:si>
-    <x:t>_Новый продукт</x:t>
-  </x:si>
-  <x:si>
-    <x:t>89</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TTTT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cat3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Подкатегория 3,1</x:t>
+    <x:t>xbgxcnbh sdrhy esty seyteart yaetya et</x:t>
   </x:si>
   <x:si>
     <x:t>11111111111111111111111111111111111</x:t>
@@ -118,28 +106,55 @@
     <x:t>333</x:t>
   </x:si>
   <x:si>
-    <x:t>Samsung</x:t>
+    <x:t>Linear</x:t>
   </x:si>
   <x:si>
     <x:t>19.12</x:t>
   </x:si>
   <x:si>
+    <x:t>111144111</x:t>
+  </x:si>
+  <x:si>
     <x:t>21212</x:t>
   </x:si>
   <x:si>
     <x:t>45535</x:t>
   </x:si>
   <x:si>
+    <x:t>Микросхемы</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DC-DC Преобразователи</x:t>
+  </x:si>
+  <x:si>
     <x:t>2332333</x:t>
   </x:si>
   <x:si>
     <x:t>233</x:t>
   </x:si>
   <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>23213</x:t>
+    <x:t>46436f</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dfgdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Intel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>464v6464v64</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5732753753</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7575757557.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ON Semiconductor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7575</x:t>
   </x:si>
   <x:si>
     <x:t>Bpvtyty</x:t>
@@ -148,7 +163,7 @@
     <x:t>99998999</x:t>
   </x:si>
   <x:si>
-    <x:t>ON</x:t>
+    <x:t>Cat2</x:t>
   </x:si>
   <x:si>
     <x:t>cat1.3</x:t>
@@ -157,7 +172,13 @@
     <x:t>asdfsadfsd</x:t>
   </x:si>
   <x:si>
-    <x:t>Brand2</x:t>
+    <x:t>Fairchild</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hdsh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>36356ertherth</x:t>
   </x:si>
   <x:si>
     <x:t>new2</x:t>
@@ -187,16 +208,22 @@
     <x:t>sgshgdfs sghsd dhsdwargt</x:t>
   </x:si>
   <x:si>
-    <x:t>Product cat4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>sgsgs4</x:t>
+    <x:t>ord</x:t>
+  </x:si>
+  <x:si>
+    <x:t>777777ord</x:t>
   </x:si>
   <x:si>
     <x:t>Product2</x:t>
   </x:si>
   <x:si>
     <x:t>9663558</x:t>
+  </x:si>
+  <x:si>
+    <x:t>rewrwe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>445225</x:t>
   </x:si>
   <x:si>
     <x:t>аа</x:t>
@@ -290,8 +317,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K18" totalsRowShown="0">
-  <x:autoFilter ref="A1:K18"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K22" totalsRowShown="0">
+  <x:autoFilter ref="A1:K22"/>
   <x:tableColumns count="11">
     <x:tableColumn id="1" name="Column1"/>
     <x:tableColumn id="2" name="Column2"/>
@@ -597,16 +624,17 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:K18"/>
+  <x:dimension ref="A1:K22"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="37.996339" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="11.996339" style="0" customWidth="1"/>
-    <x:col min="3" max="4" width="11.282054" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="17.424911" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="13.710625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="13.424911" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="23.853482" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="51.567768" style="0" customWidth="1"/>
     <x:col min="7" max="7" width="11.282054" style="0" customWidth="1"/>
     <x:col min="8" max="8" width="17.424911" style="0" customWidth="1"/>
@@ -697,6 +725,9 @@
       <x:c r="E3" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
       <x:c r="J3" s="0">
         <x:v>10</x:v>
       </x:c>
@@ -706,95 +737,89 @@
     </x:row>
     <x:row r="4" spans="1:11">
       <x:c r="A4" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="J4" s="0">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="K4" s="0">
-        <x:v>10</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:11">
       <x:c r="A5" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="J5" s="0">
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:11">
       <x:c r="A6" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="G6" s="0">
-        <x:v>123124</x:v>
-      </x:c>
       <x:c r="J6" s="0">
-        <x:v>22</x:v>
+        <x:v>2225555</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:11">
       <x:c r="A7" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="J7" s="0">
-        <x:v>2225555</x:v>
+      <x:c r="E7" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="G7" s="0">
+        <x:v>1222</x:v>
+      </x:c>
+      <x:c r="K7" s="0">
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:11">
       <x:c r="A8" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="G8" s="0">
-        <x:v>1222</x:v>
-      </x:c>
-      <x:c r="K8" s="0">
-        <x:v>12</x:v>
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="J8" s="0">
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:11">
       <x:c r="A9" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
         <x:v>25</x:v>
@@ -805,159 +830,153 @@
     </x:row>
     <x:row r="10" spans="1:11">
       <x:c r="A10" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:11">
       <x:c r="A11" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="J11" s="0">
-        <x:v>20</x:v>
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>25</x:v>
       </x:c>
       <x:c r="K11" s="0">
-        <x:v>30</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:11">
       <x:c r="A12" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
       <x:c r="J12" s="0">
-        <x:v>250</x:v>
-      </x:c>
-      <x:c r="K12" s="0">
-        <x:v>10</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:11">
       <x:c r="A13" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="B13" s="0" t="s">
+      <x:c r="C13" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="C13" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="E13" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="F13" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="G13" s="0">
-        <x:v>324</x:v>
-      </x:c>
       <x:c r="J13" s="0">
-        <x:v>444</x:v>
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K13" s="0">
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:11">
       <x:c r="A14" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="B14" s="0" t="s">
+      <x:c r="C14" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="C14" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="D14" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F14" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="G14" s="0">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="J14" s="0">
         <x:v>250</x:v>
       </x:c>
-      <x:c r="J14" s="0">
-        <x:v>50</x:v>
+      <x:c r="K14" s="0">
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:11">
       <x:c r="A15" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="B15" s="0" t="s">
-        <x:v>55</x:v>
+      <x:c r="C15" s="0" t="s">
+        <x:v>45</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
         <x:v>25</x:v>
-      </x:c>
-      <x:c r="F15" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="G15" s="0">
-        <x:v>2333</x:v>
-      </x:c>
-      <x:c r="J15" s="0">
-        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:11">
       <x:c r="A16" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="E16" s="0" t="s">
-        <x:v>25</x:v>
+      <x:c r="G16" s="0">
+        <x:v>324</x:v>
       </x:c>
       <x:c r="J16" s="0">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="K16" s="0">
-        <x:v>10</x:v>
+        <x:v>444</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:11">
       <x:c r="A17" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="B17" s="0" t="s">
+      <x:c r="C17" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="s">
         <x:v>60</x:v>
       </x:c>
-      <x:c r="E17" s="0" t="s">
-        <x:v>25</x:v>
+      <x:c r="G17" s="0">
+        <x:v>250</x:v>
       </x:c>
       <x:c r="J17" s="0">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="K17" s="0">
-        <x:v>10</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:11">
@@ -967,19 +986,87 @@
       <x:c r="B18" s="0" t="s">
         <x:v>62</x:v>
       </x:c>
-      <x:c r="C18" s="0" t="s">
+      <x:c r="E18" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="G18" s="0">
+        <x:v>2333</x:v>
+      </x:c>
+      <x:c r="J18" s="0">
+        <x:v>150</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:11">
+      <x:c r="A19" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:11">
+      <x:c r="A20" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="J20" s="0">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="K20" s="0">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:11">
+      <x:c r="A21" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="D18" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="J18" s="0">
+      <x:c r="E21" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:11">
+      <x:c r="A22" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="J22" s="0">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="K18" s="0">
+      <x:c r="K22" s="0">
         <x:v>10</x:v>
       </x:c>
     </x:row>

</xml_diff>